<commit_message>
refined cleaning and load testing
</commit_message>
<xml_diff>
--- a/Timekeeping/2019/04-19/BOLIN A 04-19.xlsx
+++ b/Timekeeping/2019/04-19/BOLIN A 04-19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ABolin\Desktop\Andrea FOLDERS\3 Office\3 Timesheets\Timesheets 2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\353-final-project\Timekeeping\2019\04-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5960E4D-47DF-4DB6-8A08-E67C1ED0C65B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62162EE-FAE7-430C-B69C-56D8D27E1FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2960" yWindow="2960" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$AJ$49</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="83">
   <si>
     <t>NAME</t>
   </si>
@@ -749,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -978,17 +984,24 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,9 +1020,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1047,9 +1060,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1082,26 +1095,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1134,26 +1130,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1333,24 +1312,24 @@
   <dimension ref="A1:GH93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AL24" sqref="AL24"/>
+      <selection activeCell="AK4" sqref="AK4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="63" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="63" customWidth="1"/>
+    <col min="1" max="1" width="5.36328125" style="63" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" style="63" customWidth="1"/>
     <col min="3" max="3" width="5" style="65" customWidth="1"/>
-    <col min="4" max="34" width="3.44140625" style="92" customWidth="1"/>
-    <col min="35" max="35" width="5.6640625" style="66" customWidth="1"/>
-    <col min="36" max="36" width="40.6640625" style="64" customWidth="1"/>
-    <col min="37" max="37" width="2.6640625" style="8" customWidth="1"/>
-    <col min="38" max="38" width="25.5546875" style="8" customWidth="1"/>
-    <col min="39" max="190" width="7.5546875" style="8" customWidth="1"/>
-    <col min="191" max="16384" width="7.5546875" style="8"/>
+    <col min="4" max="34" width="3.453125" style="92" customWidth="1"/>
+    <col min="35" max="35" width="5.6328125" style="66" customWidth="1"/>
+    <col min="36" max="36" width="40.6328125" style="64" customWidth="1"/>
+    <col min="37" max="37" width="2.6328125" style="8" customWidth="1"/>
+    <col min="38" max="38" width="25.54296875" style="8" customWidth="1"/>
+    <col min="39" max="190" width="7.54296875" style="8" customWidth="1"/>
+    <col min="191" max="16384" width="7.54296875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:190" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:190" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1369,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="P1" s="71"/>
-      <c r="Q1" s="93" t="s">
+      <c r="Q1" s="94" t="s">
         <v>1</v>
       </c>
       <c r="R1" s="73"/>
@@ -1432,37 +1411,37 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="94"/>
-      <c r="S2" s="94"/>
-      <c r="T2" s="94"/>
-      <c r="U2" s="94"/>
-      <c r="V2" s="94"/>
-      <c r="W2" s="94"/>
-      <c r="X2" s="94"/>
-      <c r="Y2" s="94"/>
-      <c r="Z2" s="94"/>
-      <c r="AA2" s="94"/>
-      <c r="AB2" s="94"/>
-      <c r="AC2" s="94"/>
-      <c r="AD2" s="94"/>
-      <c r="AE2" s="94"/>
-      <c r="AF2" s="94"/>
-      <c r="AG2" s="94"/>
-      <c r="AH2" s="94"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="97"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="97"/>
+      <c r="W2" s="97"/>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="97"/>
+      <c r="Z2" s="97"/>
+      <c r="AA2" s="97"/>
+      <c r="AB2" s="97"/>
+      <c r="AC2" s="97"/>
+      <c r="AD2" s="97"/>
+      <c r="AE2" s="97"/>
+      <c r="AF2" s="97"/>
+      <c r="AG2" s="97"/>
+      <c r="AH2" s="97"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="3"/>
@@ -1499,44 +1478,50 @@
       <c r="BP2" s="3"/>
       <c r="BQ2" s="3"/>
     </row>
-    <row r="3" spans="1:190" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:190" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="94"/>
-      <c r="S3" s="94"/>
-      <c r="T3" s="94"/>
-      <c r="U3" s="94"/>
-      <c r="V3" s="94"/>
-      <c r="W3" s="94"/>
-      <c r="X3" s="94"/>
-      <c r="Y3" s="94"/>
-      <c r="Z3" s="94"/>
-      <c r="AA3" s="94"/>
-      <c r="AB3" s="94"/>
-      <c r="AC3" s="94"/>
-      <c r="AD3" s="94"/>
-      <c r="AE3" s="94"/>
-      <c r="AF3" s="94"/>
-      <c r="AG3" s="94"/>
-      <c r="AH3" s="94"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="97"/>
+      <c r="U3" s="97"/>
+      <c r="V3" s="97"/>
+      <c r="W3" s="97"/>
+      <c r="X3" s="97"/>
+      <c r="Y3" s="97"/>
+      <c r="Z3" s="97"/>
+      <c r="AA3" s="97"/>
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="97"/>
+      <c r="AD3" s="97"/>
+      <c r="AE3" s="97"/>
+      <c r="AF3" s="97"/>
+      <c r="AG3" s="97"/>
+      <c r="AH3" s="97"/>
       <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="3"/>
+      <c r="AJ3" s="99" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
@@ -1574,37 +1559,37 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="94"/>
-      <c r="S4" s="94"/>
-      <c r="T4" s="94"/>
-      <c r="U4" s="94"/>
-      <c r="V4" s="94"/>
-      <c r="W4" s="94"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="94"/>
-      <c r="AB4" s="94"/>
-      <c r="AC4" s="94"/>
-      <c r="AD4" s="94"/>
-      <c r="AE4" s="94"/>
-      <c r="AF4" s="94"/>
-      <c r="AG4" s="94"/>
-      <c r="AH4" s="94"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="97"/>
+      <c r="T4" s="97"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97"/>
+      <c r="X4" s="97"/>
+      <c r="Y4" s="97"/>
+      <c r="Z4" s="97"/>
+      <c r="AA4" s="97"/>
+      <c r="AB4" s="97"/>
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="97"/>
+      <c r="AE4" s="97"/>
+      <c r="AF4" s="97"/>
+      <c r="AG4" s="97"/>
+      <c r="AH4" s="97"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2" t="s">
         <v>53</v>
@@ -1643,43 +1628,43 @@
       <c r="BP4" s="3"/>
       <c r="BQ4" s="3"/>
     </row>
-    <row r="5" spans="1:190" s="13" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:190" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="95"/>
-      <c r="N5" s="95"/>
-      <c r="O5" s="95"/>
-      <c r="P5" s="95"/>
-      <c r="Q5" s="95"/>
-      <c r="R5" s="95"/>
-      <c r="S5" s="95"/>
-      <c r="T5" s="95"/>
-      <c r="U5" s="95"/>
-      <c r="V5" s="95"/>
-      <c r="W5" s="95"/>
-      <c r="X5" s="95"/>
-      <c r="Y5" s="95"/>
-      <c r="Z5" s="95"/>
-      <c r="AA5" s="95"/>
-      <c r="AB5" s="95"/>
-      <c r="AC5" s="95"/>
-      <c r="AD5" s="95"/>
-      <c r="AE5" s="95"/>
-      <c r="AF5" s="95"/>
-      <c r="AG5" s="95"/>
-      <c r="AH5" s="95"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="96"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="98"/>
+      <c r="T5" s="98"/>
+      <c r="U5" s="98"/>
+      <c r="V5" s="98"/>
+      <c r="W5" s="98"/>
+      <c r="X5" s="98"/>
+      <c r="Y5" s="98"/>
+      <c r="Z5" s="98"/>
+      <c r="AA5" s="98"/>
+      <c r="AB5" s="98"/>
+      <c r="AC5" s="98"/>
+      <c r="AD5" s="98"/>
+      <c r="AE5" s="98"/>
+      <c r="AF5" s="98"/>
+      <c r="AG5" s="98"/>
+      <c r="AH5" s="98"/>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="12"/>
       <c r="AK5" s="3"/>
@@ -1837,7 +1822,7 @@
       <c r="GG5" s="8"/>
       <c r="GH5" s="8"/>
     </row>
-    <row r="6" spans="1:190" s="19" customFormat="1" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:190" s="19" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
@@ -2099,7 +2084,7 @@
       <c r="GG6" s="8"/>
       <c r="GH6" s="8"/>
     </row>
-    <row r="7" spans="1:190" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:190" ht="10.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
       <c r="C7" s="22" t="s">
@@ -2621,7 +2606,7 @@
       <c r="AG10" s="83"/>
       <c r="AH10" s="80"/>
       <c r="AI10" s="27">
-        <f t="shared" ref="AI10:AI12" si="2">SUM(D10:AH10)</f>
+        <f t="shared" ref="AI10:AI11" si="2">SUM(D10:AH10)</f>
         <v>0</v>
       </c>
       <c r="AJ10" s="28"/>
@@ -4505,131 +4490,131 @@
       </c>
       <c r="C25" s="38"/>
       <c r="D25" s="84">
-        <f>SUM(D8:D24)</f>
+        <f t="shared" ref="D25:AI25" si="6">SUM(D8:D24)</f>
         <v>7</v>
       </c>
       <c r="E25" s="84">
-        <f>SUM(E8:E24)</f>
+        <f t="shared" si="6"/>
         <v>8.5</v>
       </c>
       <c r="F25" s="84">
-        <f>SUM(F8:F24)</f>
+        <f t="shared" si="6"/>
         <v>6.5</v>
       </c>
       <c r="G25" s="84">
-        <f>SUM(G8:G24)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="H25" s="84">
-        <f>SUM(H8:H24)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I25" s="84">
-        <f>SUM(I8:I24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J25" s="84">
-        <f>SUM(J8:J24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K25" s="84">
-        <f>SUM(K8:K24)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="L25" s="84">
-        <f>SUM(L8:L24)</f>
+        <f t="shared" si="6"/>
         <v>8.5</v>
       </c>
       <c r="M25" s="84">
-        <f>SUM(M8:M24)</f>
+        <f t="shared" si="6"/>
         <v>8.5</v>
       </c>
       <c r="N25" s="84">
-        <f>SUM(N8:N24)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="O25" s="84">
-        <f>SUM(O8:O24)</f>
+        <f t="shared" si="6"/>
         <v>6.5</v>
       </c>
       <c r="P25" s="84">
-        <f>SUM(P8:P24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q25" s="84">
-        <f>SUM(Q8:Q24)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R25" s="84">
-        <f>SUM(R8:R24)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="S25" s="84">
-        <f>SUM(S8:S24)</f>
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
       <c r="T25" s="84">
-        <f>SUM(T8:T24)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="U25" s="84">
-        <f>SUM(U8:U24)</f>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="V25" s="84">
-        <f>SUM(V8:V24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W25" s="84">
-        <f>SUM(W8:W24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X25" s="84">
-        <f>SUM(X8:X24)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="Y25" s="84">
-        <f>SUM(Y8:Y24)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="Z25" s="84">
-        <f>SUM(Z8:Z24)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="AA25" s="84">
-        <f>SUM(AA8:AA24)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="AB25" s="84">
-        <f>SUM(AB8:AB24)</f>
+        <f t="shared" si="6"/>
         <v>8.5</v>
       </c>
       <c r="AC25" s="84">
-        <f>SUM(AC8:AC24)</f>
+        <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
       <c r="AD25" s="84">
-        <f>SUM(AD8:AD24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE25" s="84">
-        <f>SUM(AE8:AE24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF25" s="84">
-        <f>SUM(AF8:AF24)</f>
+        <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
       <c r="AG25" s="84">
-        <f>SUM(AG8:AG24)</f>
+        <f t="shared" si="6"/>
         <v>6.5</v>
       </c>
       <c r="AH25" s="84">
-        <f>SUM(AH8:AH24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI25" s="27">
-        <f>SUM(AI8:AI24)</f>
+        <f t="shared" si="6"/>
         <v>139.5</v>
       </c>
       <c r="AJ25" s="39"/>
@@ -5583,7 +5568,7 @@
       <c r="AG31" s="85"/>
       <c r="AH31" s="85"/>
       <c r="AI31" s="27">
-        <f t="shared" ref="AI31:AI38" si="6">SUM(D31:AH31)</f>
+        <f t="shared" ref="AI31:AI38" si="7">SUM(D31:AH31)</f>
         <v>0</v>
       </c>
       <c r="AJ31" s="43"/>
@@ -5659,7 +5644,7 @@
       <c r="AG32" s="85"/>
       <c r="AH32" s="85"/>
       <c r="AI32" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ32" s="46" t="s">
@@ -5700,7 +5685,7 @@
       <c r="BQ32" s="3"/>
     </row>
     <row r="33" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A33" s="96" t="s">
+      <c r="A33" s="93" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="45"/>
@@ -5745,7 +5730,7 @@
       <c r="AG33" s="85"/>
       <c r="AH33" s="85"/>
       <c r="AI33" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
       <c r="AJ33" s="39" t="s">
@@ -5786,7 +5771,7 @@
       <c r="BQ33" s="3"/>
     </row>
     <row r="34" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="93" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="45"/>
@@ -5827,7 +5812,7 @@
       <c r="AG34" s="85"/>
       <c r="AH34" s="85"/>
       <c r="AI34" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AJ34" s="43" t="s">
@@ -5868,7 +5853,7 @@
       <c r="BQ34" s="3"/>
     </row>
     <row r="35" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A35" s="96" t="s">
+      <c r="A35" s="93" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="45"/>
@@ -5907,7 +5892,7 @@
       <c r="AG35" s="85"/>
       <c r="AH35" s="85"/>
       <c r="AI35" s="27">
-        <f t="shared" ref="AI35:AI37" si="7">SUM(D35:AH35)</f>
+        <f t="shared" ref="AI35:AI37" si="8">SUM(D35:AH35)</f>
         <v>1</v>
       </c>
       <c r="AJ35" s="43"/>
@@ -5946,7 +5931,7 @@
       <c r="BQ35" s="3"/>
     </row>
     <row r="36" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A36" s="96" t="s">
+      <c r="A36" s="93" t="s">
         <v>76</v>
       </c>
       <c r="B36" s="45"/>
@@ -5987,7 +5972,7 @@
       <c r="AG36" s="85"/>
       <c r="AH36" s="85"/>
       <c r="AI36" s="27">
-        <f t="shared" ref="AI36" si="8">SUM(D36:AH36)</f>
+        <f t="shared" ref="AI36" si="9">SUM(D36:AH36)</f>
         <v>2</v>
       </c>
       <c r="AJ36" s="43"/>
@@ -6026,7 +6011,7 @@
       <c r="BQ36" s="3"/>
     </row>
     <row r="37" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A37" s="96" t="s">
+      <c r="A37" s="93" t="s">
         <v>69</v>
       </c>
       <c r="B37" s="45"/>
@@ -6065,7 +6050,7 @@
       <c r="AG37" s="85"/>
       <c r="AH37" s="85"/>
       <c r="AI37" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AJ37" s="43"/>
@@ -6104,7 +6089,7 @@
       <c r="BQ37" s="3"/>
     </row>
     <row r="38" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A38" s="96" t="s">
+      <c r="A38" s="93" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="45"/>
@@ -6143,7 +6128,7 @@
       <c r="AG38" s="85"/>
       <c r="AH38" s="85"/>
       <c r="AI38" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ38" s="43"/>
@@ -6192,127 +6177,127 @@
         <v>8</v>
       </c>
       <c r="E39" s="84">
-        <f t="shared" ref="E39" si="9">SUM(E25:E38)</f>
+        <f t="shared" ref="E39" si="10">SUM(E25:E38)</f>
         <v>8.5</v>
       </c>
       <c r="F39" s="84">
-        <f t="shared" ref="F39" si="10">SUM(F25:F38)</f>
+        <f t="shared" ref="F39" si="11">SUM(F25:F38)</f>
         <v>9</v>
       </c>
       <c r="G39" s="84">
-        <f t="shared" ref="G39" si="11">SUM(G25:G38)</f>
+        <f t="shared" ref="G39" si="12">SUM(G25:G38)</f>
         <v>8</v>
       </c>
       <c r="H39" s="84">
-        <f t="shared" ref="H39" si="12">SUM(H25:H38)</f>
+        <f t="shared" ref="H39" si="13">SUM(H25:H38)</f>
         <v>9</v>
       </c>
       <c r="I39" s="84">
-        <f t="shared" ref="I39" si="13">SUM(I25:I38)</f>
+        <f t="shared" ref="I39" si="14">SUM(I25:I38)</f>
         <v>0</v>
       </c>
       <c r="J39" s="84">
-        <f t="shared" ref="J39" si="14">SUM(J25:J38)</f>
+        <f t="shared" ref="J39" si="15">SUM(J25:J38)</f>
         <v>0</v>
       </c>
       <c r="K39" s="84">
-        <f t="shared" ref="K39" si="15">SUM(K25:K38)</f>
+        <f t="shared" ref="K39" si="16">SUM(K25:K38)</f>
         <v>8</v>
       </c>
       <c r="L39" s="84">
-        <f t="shared" ref="L39" si="16">SUM(L25:L38)</f>
+        <f t="shared" ref="L39" si="17">SUM(L25:L38)</f>
         <v>8.5</v>
       </c>
       <c r="M39" s="84">
-        <f t="shared" ref="M39" si="17">SUM(M25:M38)</f>
+        <f t="shared" ref="M39" si="18">SUM(M25:M38)</f>
         <v>8.5</v>
       </c>
       <c r="N39" s="84">
-        <f t="shared" ref="N39" si="18">SUM(N25:N38)</f>
+        <f t="shared" ref="N39" si="19">SUM(N25:N38)</f>
         <v>9</v>
       </c>
       <c r="O39" s="84">
-        <f t="shared" ref="O39" si="19">SUM(O25:O38)</f>
+        <f t="shared" ref="O39" si="20">SUM(O25:O38)</f>
         <v>8.5</v>
       </c>
       <c r="P39" s="84">
-        <f t="shared" ref="P39" si="20">SUM(P25:P38)</f>
+        <f t="shared" ref="P39" si="21">SUM(P25:P38)</f>
         <v>0</v>
       </c>
       <c r="Q39" s="84">
-        <f t="shared" ref="Q39" si="21">SUM(Q25:Q38)</f>
+        <f t="shared" ref="Q39" si="22">SUM(Q25:Q38)</f>
         <v>1</v>
       </c>
       <c r="R39" s="84">
-        <f t="shared" ref="R39" si="22">SUM(R25:R38)</f>
+        <f t="shared" ref="R39" si="23">SUM(R25:R38)</f>
         <v>8</v>
       </c>
       <c r="S39" s="84">
-        <f t="shared" ref="S39" si="23">SUM(S25:S38)</f>
+        <f t="shared" ref="S39" si="24">SUM(S25:S38)</f>
         <v>3.5</v>
       </c>
       <c r="T39" s="84">
-        <f t="shared" ref="T39" si="24">SUM(T25:T38)</f>
+        <f t="shared" ref="T39" si="25">SUM(T25:T38)</f>
         <v>3</v>
       </c>
       <c r="U39" s="84">
-        <f t="shared" ref="U39" si="25">SUM(U25:U38)</f>
+        <f t="shared" ref="U39" si="26">SUM(U25:U38)</f>
         <v>0.5</v>
       </c>
       <c r="V39" s="84">
-        <f t="shared" ref="V39" si="26">SUM(V25:V38)</f>
+        <f t="shared" ref="V39" si="27">SUM(V25:V38)</f>
         <v>7.5</v>
       </c>
       <c r="W39" s="84">
-        <f t="shared" ref="W39" si="27">SUM(W25:W38)</f>
+        <f t="shared" ref="W39" si="28">SUM(W25:W38)</f>
         <v>0</v>
       </c>
       <c r="X39" s="84">
-        <f t="shared" ref="X39" si="28">SUM(X25:X38)</f>
+        <f t="shared" ref="X39" si="29">SUM(X25:X38)</f>
         <v>2</v>
       </c>
       <c r="Y39" s="84">
-        <f t="shared" ref="Y39" si="29">SUM(Y25:Y38)</f>
+        <f t="shared" ref="Y39" si="30">SUM(Y25:Y38)</f>
         <v>8</v>
       </c>
       <c r="Z39" s="84">
-        <f t="shared" ref="Z39" si="30">SUM(Z25:Z38)</f>
+        <f t="shared" ref="Z39" si="31">SUM(Z25:Z38)</f>
         <v>8</v>
       </c>
       <c r="AA39" s="84">
-        <f t="shared" ref="AA39" si="31">SUM(AA25:AA38)</f>
+        <f t="shared" ref="AA39" si="32">SUM(AA25:AA38)</f>
         <v>8</v>
       </c>
       <c r="AB39" s="84">
-        <f t="shared" ref="AB39" si="32">SUM(AB25:AB38)</f>
+        <f t="shared" ref="AB39" si="33">SUM(AB25:AB38)</f>
         <v>8.5</v>
       </c>
       <c r="AC39" s="84">
-        <f t="shared" ref="AC39" si="33">SUM(AC25:AC38)</f>
+        <f t="shared" ref="AC39" si="34">SUM(AC25:AC38)</f>
         <v>9.5</v>
       </c>
       <c r="AD39" s="84">
-        <f t="shared" ref="AD39" si="34">SUM(AD25:AD38)</f>
+        <f t="shared" ref="AD39" si="35">SUM(AD25:AD38)</f>
         <v>0</v>
       </c>
       <c r="AE39" s="84">
-        <f t="shared" ref="AE39" si="35">SUM(AE25:AE38)</f>
+        <f t="shared" ref="AE39" si="36">SUM(AE25:AE38)</f>
         <v>0</v>
       </c>
       <c r="AF39" s="84">
-        <f t="shared" ref="AF39" si="36">SUM(AF25:AF38)</f>
+        <f t="shared" ref="AF39" si="37">SUM(AF25:AF38)</f>
         <v>7.5</v>
       </c>
       <c r="AG39" s="84">
-        <f t="shared" ref="AG39" si="37">SUM(AG25:AG38)</f>
+        <f t="shared" ref="AG39" si="38">SUM(AG25:AG38)</f>
         <v>8.5</v>
       </c>
       <c r="AH39" s="84">
-        <f t="shared" ref="AH39" si="38">SUM(AH25:AH38)</f>
+        <f t="shared" ref="AH39" si="39">SUM(AH25:AH38)</f>
         <v>0</v>
       </c>
       <c r="AI39" s="47">
-        <f t="shared" ref="AI39" si="39">SUM(AI25:AI38)</f>
+        <f t="shared" ref="AI39" si="40">SUM(AI25:AI38)</f>
         <v>168.5</v>
       </c>
       <c r="AJ39" s="48"/>
@@ -6421,7 +6406,7 @@
       <c r="BP40" s="3"/>
       <c r="BQ40" s="3"/>
     </row>
-    <row r="41" spans="1:69" s="3" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:69" s="3" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="49" t="s">
         <v>25</v>
       </c>
@@ -6462,7 +6447,7 @@
       <c r="AJ41" s="53"/>
       <c r="AZ41" s="4"/>
     </row>
-    <row r="42" spans="1:69" s="3" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:69" s="3" customFormat="1" ht="10.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">
         <v>26</v>
       </c>
@@ -6520,7 +6505,7 @@
       <c r="AN42" s="40"/>
       <c r="AZ42" s="4"/>
     </row>
-    <row r="43" spans="1:69" s="3" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:69" s="3" customFormat="1" ht="10" x14ac:dyDescent="0.2">
       <c r="A43" s="54" t="s">
         <v>31</v>
       </c>
@@ -6568,7 +6553,7 @@
       <c r="AK43" s="40"/>
       <c r="AZ43" s="4"/>
     </row>
-    <row r="44" spans="1:69" s="3" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:69" s="3" customFormat="1" ht="10" x14ac:dyDescent="0.2">
       <c r="A44" s="54" t="s">
         <v>35</v>
       </c>
@@ -6623,7 +6608,7 @@
       <c r="AM44" s="40"/>
       <c r="AZ44" s="4"/>
     </row>
-    <row r="45" spans="1:69" s="3" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:69" s="3" customFormat="1" ht="10" x14ac:dyDescent="0.2">
       <c r="A45" s="51" t="s">
         <v>41</v>
       </c>
@@ -6670,7 +6655,7 @@
       <c r="AJ45" s="53"/>
       <c r="AK45" s="40"/>
     </row>
-    <row r="46" spans="1:69" s="3" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:69" s="3" customFormat="1" ht="10" x14ac:dyDescent="0.2">
       <c r="A46" s="53" t="s">
         <v>45</v>
       </c>
@@ -6721,7 +6706,7 @@
       </c>
       <c r="AJ46" s="53"/>
     </row>
-    <row r="47" spans="1:69" s="3" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:69" s="3" customFormat="1" ht="10" x14ac:dyDescent="0.2">
       <c r="A47" s="53" t="s">
         <v>60</v>
       </c>
@@ -6765,7 +6750,7 @@
       <c r="AI47" s="58"/>
       <c r="AJ47" s="53"/>
     </row>
-    <row r="48" spans="1:69" s="3" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:69" s="3" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="61"/>
       <c r="B48" s="61"/>
       <c r="C48" s="61"/>
@@ -6808,7 +6793,7 @@
       </c>
       <c r="AJ48" s="53"/>
     </row>
-    <row r="49" spans="1:36" s="3" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" s="3" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="61"/>
       <c r="B49" s="61"/>
       <c r="C49" s="61"/>
@@ -7126,7 +7111,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="31">
+  <mergeCells count="30">
     <mergeCell ref="O2:O5"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
@@ -7141,7 +7126,6 @@
     <mergeCell ref="N2:N5"/>
     <mergeCell ref="AA2:AA5"/>
     <mergeCell ref="P2:P5"/>
-    <mergeCell ref="Q2:Q5"/>
     <mergeCell ref="R2:R5"/>
     <mergeCell ref="S2:S5"/>
     <mergeCell ref="T2:T5"/>

</xml_diff>